<commit_message>
Plan aktuallisiert, gemäß Besprechung
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="24000" windowHeight="9870"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="15360" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="71">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -265,10 +265,13 @@
     <t>GUI</t>
   </si>
   <si>
-    <t>tbd</t>
-  </si>
-  <si>
-    <t>Marc</t>
+    <t>Adriana, Natalja</t>
+  </si>
+  <si>
+    <t>Ralf</t>
+  </si>
+  <si>
+    <t>Marc, Ralf, Katrin, Johannes</t>
   </si>
 </sst>
 </file>
@@ -695,16 +698,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="33.75" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.25" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="10.5" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="5" width="11.25" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="10.5" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="10.5" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="8" max="8" width="39.75" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="9" max="9" width="64.125" hidden="1" customWidth="1" outlineLevel="2"/>
@@ -2463,15 +2466,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2504,7 +2507,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2514,13 +2517,19 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planung aktuallisiert - ER-Modell entfallen
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Fallstudie\Projektmanagement\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="15360" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
     <sheet name="Teams" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A13:AM32"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="72">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -70,9 +66,6 @@
     <t>Design Guide erstellen</t>
   </si>
   <si>
-    <t>ER Modell erstellen</t>
-  </si>
-  <si>
     <t>Aktivitätsdiagram erstellen</t>
   </si>
   <si>
@@ -272,6 +265,12 @@
   </si>
   <si>
     <t>Marc, Ralf, Katrin, Johannes</t>
+  </si>
+  <si>
+    <t>ready4review</t>
+  </si>
+  <si>
+    <t>in Gruppe abgestimmt</t>
   </si>
 </sst>
 </file>
@@ -402,21 +401,21 @@
   <dxfs count="2">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -696,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR35"/>
+  <dimension ref="A1:AR37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -708,7 +707,7 @@
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.25" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="10.5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="10.5" hidden="1" customWidth="1" outlineLevel="2"/>
+    <col min="7" max="7" width="11.625" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="8" max="8" width="39.75" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="9" max="9" width="64.125" hidden="1" customWidth="1" outlineLevel="2"/>
     <col min="10" max="10" width="3.125" customWidth="1" collapsed="1"/>
@@ -717,13 +716,13 @@
   <sheetData>
     <row r="1" spans="1:44">
       <c r="J1" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
@@ -758,31 +757,31 @@
     </row>
     <row r="2" spans="1:44">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="5">
         <v>41544</v>
@@ -890,15 +889,15 @@
         <v>41578</v>
       </c>
     </row>
-    <row r="3" spans="1:44" outlineLevel="1">
+    <row r="3" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2">
         <v>41544</v>
@@ -907,13 +906,13 @@
         <v>41544</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="9"/>
@@ -936,15 +935,15 @@
       <c r="AQ3" s="11"/>
       <c r="AR3" s="11"/>
     </row>
-    <row r="4" spans="1:44" outlineLevel="1">
+    <row r="4" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
         <v>41544</v>
@@ -953,31 +952,25 @@
         <v>41551</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>71</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4" t="s">
-        <v>60</v>
-      </c>
-      <c r="N4" t="s">
-        <v>60</v>
-      </c>
-      <c r="O4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="9"/>
@@ -998,12 +991,12 @@
       <c r="AQ4" s="11"/>
       <c r="AR4" s="11"/>
     </row>
-    <row r="5" spans="1:44" outlineLevel="1">
+    <row r="5" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -1015,31 +1008,31 @@
         <v>41551</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="9"/>
@@ -1060,43 +1053,15 @@
       <c r="AQ5" s="11"/>
       <c r="AR5" s="11"/>
     </row>
-    <row r="6" spans="1:44" outlineLevel="1">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2">
-        <v>41551</v>
-      </c>
-      <c r="F6" s="2">
-        <v>41555</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
+    <row r="6" spans="1:44" customFormat="1">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="J6" s="11"/>
       <c r="K6" s="7"/>
       <c r="L6" s="9"/>
-      <c r="Q6" t="s">
-        <v>60</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S6" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="T6" t="s">
-        <v>60</v>
-      </c>
-      <c r="U6" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="R6" s="7"/>
+      <c r="S6" s="9"/>
+      <c r="U6" s="11"/>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="11"/>
@@ -1113,15 +1078,33 @@
       <c r="AQ6" s="11"/>
       <c r="AR6" s="11"/>
     </row>
-    <row r="7" spans="1:44">
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+    <row r="7" spans="1:44" customFormat="1">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="2">
+        <v>41555</v>
+      </c>
+      <c r="F7" s="2">
+        <v>41555</v>
+      </c>
       <c r="J7" s="11"/>
       <c r="K7" s="7"/>
       <c r="L7" s="9"/>
+      <c r="Q7" t="s">
+        <v>58</v>
+      </c>
       <c r="R7" s="7"/>
       <c r="S7" s="9"/>
-      <c r="U7" s="11"/>
+      <c r="U7" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="11"/>
@@ -1138,30 +1121,13 @@
       <c r="AQ7" s="11"/>
       <c r="AR7" s="11"/>
     </row>
-    <row r="8" spans="1:44">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="2">
-        <v>41555</v>
-      </c>
-      <c r="F8" s="2">
-        <v>41555</v>
-      </c>
+    <row r="8" spans="1:44" customFormat="1">
       <c r="J8" s="11"/>
       <c r="K8" s="7"/>
       <c r="L8" s="9"/>
       <c r="R8" s="7"/>
       <c r="S8" s="9"/>
-      <c r="U8" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="U8" s="11"/>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
       <c r="X8" s="11"/>
@@ -1178,15 +1144,64 @@
       <c r="AQ8" s="11"/>
       <c r="AR8" s="11"/>
     </row>
-    <row r="9" spans="1:44">
+    <row r="9" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2">
+        <v>41555</v>
+      </c>
+      <c r="F9" s="2">
+        <v>41557</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>39</v>
+      </c>
       <c r="J9" s="11"/>
       <c r="K9" s="7"/>
       <c r="L9" s="9"/>
-      <c r="R9" s="7"/>
-      <c r="S9" s="9"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
+      <c r="M9" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O9" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="W9" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="X9" s="11"/>
       <c r="Y9" s="7"/>
       <c r="Z9" s="9"/>
@@ -1201,15 +1216,15 @@
       <c r="AQ9" s="11"/>
       <c r="AR9" s="11"/>
     </row>
-    <row r="10" spans="1:44" outlineLevel="1">
+    <row r="10" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2">
         <v>41555</v>
@@ -1218,7 +1233,7 @@
         <v>41556</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="7"/>
@@ -1226,10 +1241,10 @@
       <c r="R10" s="7"/>
       <c r="S10" s="9"/>
       <c r="U10" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
@@ -1246,15 +1261,15 @@
       <c r="AQ10" s="11"/>
       <c r="AR10" s="11"/>
     </row>
-    <row r="11" spans="1:44" outlineLevel="1">
+    <row r="11" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2">
         <v>41555</v>
@@ -1263,7 +1278,7 @@
         <v>41557</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="7"/>
@@ -1271,13 +1286,13 @@
       <c r="R11" s="7"/>
       <c r="S11" s="9"/>
       <c r="U11" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W11" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X11" s="11"/>
       <c r="Y11" s="7"/>
@@ -1293,9 +1308,9 @@
       <c r="AQ11" s="11"/>
       <c r="AR11" s="11"/>
     </row>
-    <row r="12" spans="1:44" outlineLevel="1">
+    <row r="12" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
@@ -1318,13 +1333,13 @@
       <c r="R12" s="7"/>
       <c r="S12" s="9"/>
       <c r="U12" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W12" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X12" s="11"/>
       <c r="Y12" s="7"/>
@@ -1340,39 +1355,15 @@
       <c r="AQ12" s="11"/>
       <c r="AR12" s="11"/>
     </row>
-    <row r="13" spans="1:44" outlineLevel="1">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2">
-        <v>41555</v>
-      </c>
-      <c r="F13" s="2">
-        <v>41557</v>
-      </c>
-      <c r="H13" t="s">
-        <v>41</v>
-      </c>
+    <row r="13" spans="1:44" customFormat="1">
       <c r="J13" s="11"/>
       <c r="K13" s="7"/>
       <c r="L13" s="9"/>
       <c r="R13" s="7"/>
       <c r="S13" s="9"/>
-      <c r="U13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="V13" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="W13" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
       <c r="X13" s="11"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="9"/>
@@ -1387,7 +1378,22 @@
       <c r="AQ13" s="11"/>
       <c r="AR13" s="11"/>
     </row>
-    <row r="14" spans="1:44">
+    <row r="14" spans="1:44" customFormat="1">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2">
+        <v>41557</v>
+      </c>
+      <c r="F14" s="2">
+        <v>41557</v>
+      </c>
       <c r="J14" s="11"/>
       <c r="K14" s="7"/>
       <c r="L14" s="9"/>
@@ -1395,7 +1401,9 @@
       <c r="S14" s="9"/>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
+      <c r="W14" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="X14" s="11"/>
       <c r="Y14" s="7"/>
       <c r="Z14" s="9"/>
@@ -1410,21 +1418,24 @@
       <c r="AQ14" s="11"/>
       <c r="AR14" s="11"/>
     </row>
-    <row r="15" spans="1:44">
+    <row r="15" spans="1:44" customFormat="1">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="2">
         <v>41557</v>
       </c>
       <c r="F15" s="2">
         <v>41557</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="7"/>
@@ -1434,7 +1445,7 @@
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X15" s="11"/>
       <c r="Y15" s="7"/>
@@ -1450,25 +1461,7 @@
       <c r="AQ15" s="11"/>
       <c r="AR15" s="11"/>
     </row>
-    <row r="16" spans="1:44">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="2">
-        <v>41557</v>
-      </c>
-      <c r="F16" s="2">
-        <v>41557</v>
-      </c>
-      <c r="H16" t="s">
-        <v>48</v>
-      </c>
+    <row r="16" spans="1:44" customFormat="1">
       <c r="J16" s="11"/>
       <c r="K16" s="7"/>
       <c r="L16" s="9"/>
@@ -1476,9 +1469,7 @@
       <c r="S16" s="9"/>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
-      <c r="W16" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="W16" s="11"/>
       <c r="X16" s="11"/>
       <c r="Y16" s="7"/>
       <c r="Z16" s="9"/>
@@ -1493,7 +1484,25 @@
       <c r="AQ16" s="11"/>
       <c r="AR16" s="11"/>
     </row>
-    <row r="17" spans="1:44">
+    <row r="17" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2">
+        <v>41557</v>
+      </c>
+      <c r="F17" s="2">
+        <v>41557</v>
+      </c>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
       <c r="J17" s="11"/>
       <c r="K17" s="7"/>
       <c r="L17" s="9"/>
@@ -1501,7 +1510,9 @@
       <c r="S17" s="9"/>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="W17" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="X17" s="11"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="9"/>
@@ -1516,24 +1527,21 @@
       <c r="AQ17" s="11"/>
       <c r="AR17" s="11"/>
     </row>
-    <row r="18" spans="1:44" outlineLevel="1">
+    <row r="18" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2">
         <v>41557</v>
       </c>
       <c r="F18" s="2">
-        <v>41557</v>
-      </c>
-      <c r="H18" t="s">
-        <v>42</v>
+        <v>41562</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="7"/>
@@ -1543,12 +1551,23 @@
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
       <c r="W18" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="7"/>
-      <c r="Z18" s="9"/>
-      <c r="AB18" s="11"/>
+        <v>59</v>
+      </c>
+      <c r="X18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z18" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB18" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AF18" s="7"/>
       <c r="AG18" s="9"/>
       <c r="AI18" s="11"/>
@@ -1559,9 +1578,9 @@
       <c r="AQ18" s="11"/>
       <c r="AR18" s="11"/>
     </row>
-    <row r="19" spans="1:44" outlineLevel="1">
+    <row r="19" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>16</v>
@@ -1583,22 +1602,22 @@
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y19" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB19" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF19" s="7"/>
       <c r="AG19" s="9"/>
@@ -1610,15 +1629,15 @@
       <c r="AQ19" s="11"/>
       <c r="AR19" s="11"/>
     </row>
-    <row r="20" spans="1:44" outlineLevel="1">
+    <row r="20" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2">
         <v>41557</v>
@@ -1634,22 +1653,22 @@
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y20" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z20" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF20" s="7"/>
       <c r="AG20" s="9"/>
@@ -1661,15 +1680,15 @@
       <c r="AQ20" s="11"/>
       <c r="AR20" s="11"/>
     </row>
-    <row r="21" spans="1:44" outlineLevel="1">
+    <row r="21" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2">
         <v>41557</v>
@@ -1685,22 +1704,22 @@
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
       <c r="W21" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X21" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z21" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB21" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF21" s="7"/>
       <c r="AG21" s="9"/>
@@ -1712,15 +1731,15 @@
       <c r="AQ21" s="11"/>
       <c r="AR21" s="11"/>
     </row>
-    <row r="22" spans="1:44" outlineLevel="1">
+    <row r="22" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E22" s="2">
         <v>41557</v>
@@ -1736,22 +1755,22 @@
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
       <c r="W22" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X22" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y22" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z22" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB22" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF22" s="7"/>
       <c r="AG22" s="9"/>
@@ -1763,15 +1782,15 @@
       <c r="AQ22" s="11"/>
       <c r="AR22" s="11"/>
     </row>
-    <row r="23" spans="1:44" outlineLevel="1">
+    <row r="23" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E23" s="2">
         <v>41557</v>
@@ -1787,22 +1806,22 @@
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
       <c r="W23" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X23" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y23" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z23" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB23" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF23" s="7"/>
       <c r="AG23" s="9"/>
@@ -1814,18 +1833,18 @@
       <c r="AQ23" s="11"/>
       <c r="AR23" s="11"/>
     </row>
-    <row r="24" spans="1:44" outlineLevel="1">
+    <row r="24" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="2">
-        <v>41557</v>
+        <v>41562</v>
       </c>
       <c r="F24" s="2">
         <v>41562</v>
@@ -1837,23 +1856,12 @@
       <c r="S24" s="9"/>
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
-      <c r="W24" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="X24" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y24" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z24" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>60</v>
-      </c>
+      <c r="W24" s="11"/>
+      <c r="X24" s="11"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="9"/>
       <c r="AB24" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AF24" s="7"/>
       <c r="AG24" s="9"/>
@@ -1865,12 +1873,12 @@
       <c r="AQ24" s="11"/>
       <c r="AR24" s="11"/>
     </row>
-    <row r="25" spans="1:44" outlineLevel="1">
+    <row r="25" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
@@ -1879,7 +1887,7 @@
         <v>41562</v>
       </c>
       <c r="F25" s="2">
-        <v>41562</v>
+        <v>41569</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="7"/>
@@ -1895,8 +1903,21 @@
       <c r="AB25" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AF25" s="7"/>
-      <c r="AG25" s="9"/>
+      <c r="AC25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG25" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="AI25" s="11"/>
       <c r="AM25" s="7"/>
       <c r="AN25" s="9"/>
@@ -1905,22 +1926,7 @@
       <c r="AQ25" s="11"/>
       <c r="AR25" s="11"/>
     </row>
-    <row r="26" spans="1:44" outlineLevel="1">
-      <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="2">
-        <v>41562</v>
-      </c>
-      <c r="F26" s="2">
-        <v>41569</v>
-      </c>
+    <row r="26" spans="1:44" customFormat="1">
       <c r="J26" s="11"/>
       <c r="K26" s="7"/>
       <c r="L26" s="9"/>
@@ -1932,24 +1938,9 @@
       <c r="X26" s="11"/>
       <c r="Y26" s="7"/>
       <c r="Z26" s="9"/>
-      <c r="AB26" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF26" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG26" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="AB26" s="11"/>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="9"/>
       <c r="AI26" s="11"/>
       <c r="AM26" s="7"/>
       <c r="AN26" s="9"/>
@@ -1958,7 +1949,22 @@
       <c r="AQ26" s="11"/>
       <c r="AR26" s="11"/>
     </row>
-    <row r="27" spans="1:44">
+    <row r="27" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="2">
+        <v>41562</v>
+      </c>
+      <c r="F27" s="2">
+        <v>41577</v>
+      </c>
       <c r="J27" s="11"/>
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
@@ -1970,26 +1976,65 @@
       <c r="X27" s="11"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="9"/>
-      <c r="AB27" s="11"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="9"/>
-      <c r="AI27" s="11"/>
-      <c r="AM27" s="7"/>
-      <c r="AN27" s="9"/>
-      <c r="AO27" s="11"/>
-      <c r="AP27" s="11"/>
-      <c r="AQ27" s="11"/>
+      <c r="AB27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG27" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM27" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN27" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP27" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ27" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AR27" s="11"/>
     </row>
-    <row r="28" spans="1:44" outlineLevel="1">
+    <row r="28" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E28" s="2">
         <v>41562</v>
@@ -2009,67 +2054,67 @@
       <c r="Y28" s="7"/>
       <c r="Z28" s="9"/>
       <c r="AB28" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF28" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AG28" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI28" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AK28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM28" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN28" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO28" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP28" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ28" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AR28" s="11"/>
     </row>
-    <row r="29" spans="1:44" outlineLevel="1">
+    <row r="29" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E29" s="2">
-        <v>41562</v>
+        <v>41577</v>
       </c>
       <c r="F29" s="2">
         <v>41577</v>
@@ -2085,68 +2130,31 @@
       <c r="X29" s="11"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="9"/>
-      <c r="AB29" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG29" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI29" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL29" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM29" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN29" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO29" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP29" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="AB29" s="11"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="9"/>
+      <c r="AI29" s="11"/>
+      <c r="AM29" s="7"/>
+      <c r="AN29" s="9"/>
+      <c r="AO29" s="11"/>
+      <c r="AP29" s="11"/>
       <c r="AQ29" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AR29" s="11"/>
     </row>
-    <row r="30" spans="1:44" outlineLevel="1">
+    <row r="30" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E30" s="2">
-        <v>41577</v>
+        <v>41562</v>
       </c>
       <c r="F30" s="2">
         <v>41577</v>
@@ -2162,35 +2170,59 @@
       <c r="X30" s="11"/>
       <c r="Y30" s="7"/>
       <c r="Z30" s="9"/>
-      <c r="AB30" s="11"/>
-      <c r="AF30" s="7"/>
-      <c r="AG30" s="9"/>
-      <c r="AI30" s="11"/>
-      <c r="AM30" s="7"/>
-      <c r="AN30" s="9"/>
-      <c r="AO30" s="11"/>
-      <c r="AP30" s="11"/>
+      <c r="AB30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM30" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO30" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP30" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AQ30" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AR30" s="11"/>
     </row>
-    <row r="31" spans="1:44" outlineLevel="1">
-      <c r="A31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="2">
-        <v>41562</v>
-      </c>
-      <c r="F31" s="2">
-        <v>41577</v>
-      </c>
+    <row r="31" spans="1:44" customFormat="1">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
       <c r="J31" s="11"/>
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
@@ -2202,258 +2234,197 @@
       <c r="X31" s="11"/>
       <c r="Y31" s="7"/>
       <c r="Z31" s="9"/>
-      <c r="AB31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG31" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL31" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN31" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP31" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AQ31" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="AB31" s="11"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="9"/>
+      <c r="AI31" s="11"/>
+      <c r="AM31" s="7"/>
+      <c r="AN31" s="9"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="11"/>
+      <c r="AQ31" s="11"/>
       <c r="AR31" s="11"/>
     </row>
-    <row r="32" spans="1:44">
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="9"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="9"/>
-      <c r="U32" s="11"/>
-      <c r="V32" s="11"/>
-      <c r="W32" s="11"/>
-      <c r="X32" s="11"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="9"/>
-      <c r="AB32" s="11"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="9"/>
-      <c r="AI32" s="11"/>
-      <c r="AM32" s="7"/>
-      <c r="AN32" s="9"/>
-      <c r="AO32" s="11"/>
-      <c r="AP32" s="11"/>
-      <c r="AQ32" s="11"/>
+    <row r="32" spans="1:44" customFormat="1">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="2">
+        <v>41544</v>
+      </c>
+      <c r="F32" s="2">
+        <v>41577</v>
+      </c>
+      <c r="I32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M32" t="s">
+        <v>59</v>
+      </c>
+      <c r="N32" t="s">
+        <v>59</v>
+      </c>
+      <c r="O32" t="s">
+        <v>59</v>
+      </c>
+      <c r="P32" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>59</v>
+      </c>
+      <c r="R32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T32" t="s">
+        <v>59</v>
+      </c>
+      <c r="U32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="W32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP32" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ32" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AR32" s="11"/>
     </row>
-    <row r="33" spans="1:44">
+    <row r="33" spans="1:44" customFormat="1">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E33" s="2">
-        <v>41544</v>
+        <v>41577</v>
       </c>
       <c r="F33" s="2">
         <v>41577</v>
       </c>
-      <c r="I33" t="s">
-        <v>56</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="L33" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="M33" t="s">
-        <v>60</v>
-      </c>
-      <c r="N33" t="s">
-        <v>60</v>
-      </c>
-      <c r="O33" t="s">
-        <v>60</v>
-      </c>
-      <c r="P33" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>60</v>
-      </c>
-      <c r="R33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="S33" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="T33" t="s">
-        <v>60</v>
-      </c>
-      <c r="U33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="V33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="W33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="X33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z33" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AB33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG33" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL33" t="s">
-        <v>60</v>
-      </c>
-      <c r="AM33" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="AN33" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="AO33" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="AP33" s="11" t="s">
-        <v>60</v>
-      </c>
+      <c r="J33" s="11"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="9"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="9"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="9"/>
+      <c r="AB33" s="11"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="9"/>
+      <c r="AI33" s="11"/>
+      <c r="AM33" s="7"/>
+      <c r="AN33" s="9"/>
+      <c r="AO33" s="11"/>
+      <c r="AP33" s="11"/>
       <c r="AQ33" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AR33" s="11"/>
     </row>
-    <row r="34" spans="1:44">
-      <c r="A34" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E34" s="2">
-        <v>41577</v>
-      </c>
-      <c r="F34" s="2">
-        <v>41577</v>
-      </c>
+    <row r="34" spans="1:44" customFormat="1">
       <c r="J34" s="11"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="9"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="9"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="7"/>
-      <c r="Z34" s="9"/>
-      <c r="AB34" s="11"/>
-      <c r="AF34" s="7"/>
-      <c r="AG34" s="9"/>
-      <c r="AI34" s="11"/>
-      <c r="AM34" s="7"/>
-      <c r="AN34" s="9"/>
-      <c r="AO34" s="11"/>
-      <c r="AP34" s="11"/>
-      <c r="AQ34" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AR34" s="11"/>
-    </row>
-    <row r="35" spans="1:44">
-      <c r="J35" s="11"/>
-    </row>
+    </row>
+    <row r="35" spans="1:44" customFormat="1"/>
+    <row r="36" spans="1:44" customFormat="1"/>
+    <row r="37" spans="1:44" customFormat="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:AR1"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:AQ34">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="J3:AQ33">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"m"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2466,7 +2437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2479,57 +2450,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>67</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aufgabe "Pflichtenheft" hinzugefügt, Status updated
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16335" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="74">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -267,10 +267,16 @@
     <t>Marc, Ralf, Katrin, Johannes</t>
   </si>
   <si>
-    <t>ready4review</t>
-  </si>
-  <si>
     <t>in Gruppe abgestimmt</t>
+  </si>
+  <si>
+    <t>Pflichtenheft erstellen</t>
+  </si>
+  <si>
+    <t>Review Gruppe</t>
+  </si>
+  <si>
+    <t>Anforderungen und deren Lösungen, inkl. Aufwandsschätzung</t>
   </si>
 </sst>
 </file>
@@ -695,23 +701,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR37"/>
+  <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="33.75" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="10.5" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="11.625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="8" max="8" width="39.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="64.125" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="10" max="10" width="3.125" customWidth="1" collapsed="1"/>
-    <col min="11" max="44" width="3.125" customWidth="1"/>
+    <col min="4" max="5" width="11.25" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1" outlineLevel="2"/>
+    <col min="8" max="8" width="39.75" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="9" width="64.125" customWidth="1" outlineLevel="2"/>
+    <col min="10" max="44" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44">
@@ -951,14 +956,14 @@
       <c r="F4" s="2">
         <v>41551</v>
       </c>
-      <c r="G4" t="s">
-        <v>70</v>
+      <c r="G4" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="H4" t="s">
         <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>59</v>
@@ -1007,8 +1012,8 @@
       <c r="F5" s="2">
         <v>41551</v>
       </c>
-      <c r="G5" t="s">
-        <v>48</v>
+      <c r="G5" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="H5" t="s">
         <v>37</v>
@@ -1355,7 +1360,28 @@
       <c r="AQ12" s="11"/>
       <c r="AR12" s="11"/>
     </row>
-    <row r="13" spans="1:44" customFormat="1">
+    <row r="13" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2">
+        <v>41557</v>
+      </c>
+      <c r="F13" s="2">
+        <v>41557</v>
+      </c>
+      <c r="H13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" t="s">
+        <v>73</v>
+      </c>
       <c r="J13" s="11"/>
       <c r="K13" s="7"/>
       <c r="L13" s="9"/>
@@ -1363,7 +1389,9 @@
       <c r="S13" s="9"/>
       <c r="U13" s="11"/>
       <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
+      <c r="W13" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="X13" s="11"/>
       <c r="Y13" s="7"/>
       <c r="Z13" s="9"/>
@@ -1379,21 +1407,6 @@
       <c r="AR13" s="11"/>
     </row>
     <row r="14" spans="1:44" customFormat="1">
-      <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="2">
-        <v>41557</v>
-      </c>
-      <c r="F14" s="2">
-        <v>41557</v>
-      </c>
       <c r="J14" s="11"/>
       <c r="K14" s="7"/>
       <c r="L14" s="9"/>
@@ -1401,9 +1414,7 @@
       <c r="S14" s="9"/>
       <c r="U14" s="11"/>
       <c r="V14" s="11"/>
-      <c r="W14" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="W14" s="11"/>
       <c r="X14" s="11"/>
       <c r="Y14" s="7"/>
       <c r="Z14" s="9"/>
@@ -1423,7 +1434,7 @@
         <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
@@ -1433,9 +1444,6 @@
       </c>
       <c r="F15" s="2">
         <v>41557</v>
-      </c>
-      <c r="H15" t="s">
-        <v>47</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="7"/>
@@ -1462,6 +1470,24 @@
       <c r="AR15" s="11"/>
     </row>
     <row r="16" spans="1:44" customFormat="1">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2">
+        <v>41557</v>
+      </c>
+      <c r="F16" s="2">
+        <v>41557</v>
+      </c>
+      <c r="H16" t="s">
+        <v>47</v>
+      </c>
       <c r="J16" s="11"/>
       <c r="K16" s="7"/>
       <c r="L16" s="9"/>
@@ -1469,7 +1495,9 @@
       <c r="S16" s="9"/>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
+      <c r="W16" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="X16" s="11"/>
       <c r="Y16" s="7"/>
       <c r="Z16" s="9"/>
@@ -1484,25 +1512,7 @@
       <c r="AQ16" s="11"/>
       <c r="AR16" s="11"/>
     </row>
-    <row r="17" spans="1:44" customFormat="1" outlineLevel="1">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="2">
-        <v>41557</v>
-      </c>
-      <c r="F17" s="2">
-        <v>41557</v>
-      </c>
-      <c r="H17" t="s">
-        <v>41</v>
-      </c>
+    <row r="17" spans="1:44" customFormat="1">
       <c r="J17" s="11"/>
       <c r="K17" s="7"/>
       <c r="L17" s="9"/>
@@ -1510,9 +1520,7 @@
       <c r="S17" s="9"/>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
-      <c r="W17" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="W17" s="11"/>
       <c r="X17" s="11"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="9"/>
@@ -1532,7 +1540,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1541,7 +1549,10 @@
         <v>41557</v>
       </c>
       <c r="F18" s="2">
-        <v>41562</v>
+        <v>41557</v>
+      </c>
+      <c r="H18" t="s">
+        <v>41</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="7"/>
@@ -1553,21 +1564,10 @@
       <c r="W18" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="X18" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z18" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA18" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB18" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="X18" s="11"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="9"/>
+      <c r="AB18" s="11"/>
       <c r="AF18" s="7"/>
       <c r="AG18" s="9"/>
       <c r="AI18" s="11"/>
@@ -1583,10 +1583,10 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2">
         <v>41557</v>
@@ -1634,10 +1634,10 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E20" s="2">
         <v>41557</v>
@@ -1685,10 +1685,10 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E21" s="2">
         <v>41557</v>
@@ -1736,10 +1736,10 @@
         <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E22" s="2">
         <v>41557</v>
@@ -1787,7 +1787,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1838,13 +1838,13 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="2">
-        <v>41562</v>
+        <v>41557</v>
       </c>
       <c r="F24" s="2">
         <v>41562</v>
@@ -1856,12 +1856,23 @@
       <c r="S24" s="9"/>
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="7"/>
-      <c r="Z24" s="9"/>
+      <c r="W24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X24" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y24" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z24" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>59</v>
+      </c>
       <c r="AB24" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AF24" s="7"/>
       <c r="AG24" s="9"/>
@@ -1878,16 +1889,16 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="2">
         <v>41562</v>
       </c>
       <c r="F25" s="2">
-        <v>41569</v>
+        <v>41562</v>
       </c>
       <c r="J25" s="11"/>
       <c r="K25" s="7"/>
@@ -1901,23 +1912,10 @@
       <c r="Y25" s="7"/>
       <c r="Z25" s="9"/>
       <c r="AB25" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE25" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF25" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG25" s="9" t="s">
-        <v>59</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="9"/>
       <c r="AI25" s="11"/>
       <c r="AM25" s="7"/>
       <c r="AN25" s="9"/>
@@ -1926,7 +1924,22 @@
       <c r="AQ25" s="11"/>
       <c r="AR25" s="11"/>
     </row>
-    <row r="26" spans="1:44" customFormat="1">
+    <row r="26" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="2">
+        <v>41562</v>
+      </c>
+      <c r="F26" s="2">
+        <v>41569</v>
+      </c>
       <c r="J26" s="11"/>
       <c r="K26" s="7"/>
       <c r="L26" s="9"/>
@@ -1938,9 +1951,24 @@
       <c r="X26" s="11"/>
       <c r="Y26" s="7"/>
       <c r="Z26" s="9"/>
-      <c r="AB26" s="11"/>
-      <c r="AF26" s="7"/>
-      <c r="AG26" s="9"/>
+      <c r="AB26" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF26" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG26" s="9" t="s">
+        <v>59</v>
+      </c>
       <c r="AI26" s="11"/>
       <c r="AM26" s="7"/>
       <c r="AN26" s="9"/>
@@ -1949,22 +1977,7 @@
       <c r="AQ26" s="11"/>
       <c r="AR26" s="11"/>
     </row>
-    <row r="27" spans="1:44" customFormat="1" outlineLevel="1">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" t="s">
-        <v>13</v>
-      </c>
-      <c r="E27" s="2">
-        <v>41562</v>
-      </c>
-      <c r="F27" s="2">
-        <v>41577</v>
-      </c>
+    <row r="27" spans="1:44" customFormat="1">
       <c r="J27" s="11"/>
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
@@ -1976,54 +1989,15 @@
       <c r="X27" s="11"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="9"/>
-      <c r="AB27" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI27" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL27" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM27" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN27" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO27" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP27" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ27" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="AB27" s="11"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="9"/>
+      <c r="AI27" s="11"/>
+      <c r="AM27" s="7"/>
+      <c r="AN27" s="9"/>
+      <c r="AO27" s="11"/>
+      <c r="AP27" s="11"/>
+      <c r="AQ27" s="11"/>
       <c r="AR27" s="11"/>
     </row>
     <row r="28" spans="1:44" customFormat="1" outlineLevel="1">
@@ -2031,7 +2005,7 @@
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -2108,13 +2082,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="2">
-        <v>41577</v>
+        <v>41562</v>
       </c>
       <c r="F29" s="2">
         <v>41577</v>
@@ -2130,14 +2104,51 @@
       <c r="X29" s="11"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="9"/>
-      <c r="AB29" s="11"/>
-      <c r="AF29" s="7"/>
-      <c r="AG29" s="9"/>
-      <c r="AI29" s="11"/>
-      <c r="AM29" s="7"/>
-      <c r="AN29" s="9"/>
-      <c r="AO29" s="11"/>
-      <c r="AP29" s="11"/>
+      <c r="AB29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL29" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP29" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AQ29" s="11" t="s">
         <v>59</v>
       </c>
@@ -2148,13 +2159,13 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
       <c r="E30" s="2">
-        <v>41562</v>
+        <v>41577</v>
       </c>
       <c r="F30" s="2">
         <v>41577</v>
@@ -2170,59 +2181,35 @@
       <c r="X30" s="11"/>
       <c r="Y30" s="7"/>
       <c r="Z30" s="9"/>
-      <c r="AB30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG30" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL30" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM30" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN30" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP30" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="AB30" s="11"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="9"/>
+      <c r="AI30" s="11"/>
+      <c r="AM30" s="7"/>
+      <c r="AN30" s="9"/>
+      <c r="AO30" s="11"/>
+      <c r="AP30" s="11"/>
       <c r="AQ30" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AR30" s="11"/>
     </row>
-    <row r="31" spans="1:44" customFormat="1">
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+    <row r="31" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="2">
+        <v>41562</v>
+      </c>
+      <c r="F31" s="2">
+        <v>41577</v>
+      </c>
       <c r="J31" s="11"/>
       <c r="K31" s="7"/>
       <c r="L31" s="9"/>
@@ -2234,138 +2221,79 @@
       <c r="X31" s="11"/>
       <c r="Y31" s="7"/>
       <c r="Z31" s="9"/>
-      <c r="AB31" s="11"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="9"/>
-      <c r="AI31" s="11"/>
-      <c r="AM31" s="7"/>
-      <c r="AN31" s="9"/>
-      <c r="AO31" s="11"/>
-      <c r="AP31" s="11"/>
-      <c r="AQ31" s="11"/>
+      <c r="AB31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN31" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP31" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AQ31" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="AR31" s="11"/>
     </row>
     <row r="32" spans="1:44" customFormat="1">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="B32" t="s">
-        <v>25</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" s="2">
-        <v>41544</v>
-      </c>
-      <c r="F32" s="2">
-        <v>41577</v>
-      </c>
-      <c r="I32" t="s">
-        <v>55</v>
-      </c>
-      <c r="J32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M32" t="s">
-        <v>59</v>
-      </c>
-      <c r="N32" t="s">
-        <v>59</v>
-      </c>
-      <c r="O32" t="s">
-        <v>59</v>
-      </c>
-      <c r="P32" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>59</v>
-      </c>
-      <c r="R32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="T32" t="s">
-        <v>59</v>
-      </c>
-      <c r="U32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="W32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL32" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM32" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ32" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="9"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="9"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="9"/>
+      <c r="AB32" s="11"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="9"/>
+      <c r="AI32" s="11"/>
+      <c r="AM32" s="7"/>
+      <c r="AN32" s="9"/>
+      <c r="AO32" s="11"/>
+      <c r="AP32" s="11"/>
+      <c r="AQ32" s="11"/>
       <c r="AR32" s="11"/>
     </row>
     <row r="33" spans="1:44" customFormat="1">
@@ -2373,53 +2301,176 @@
         <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="E33" s="2">
-        <v>41577</v>
+        <v>41544</v>
       </c>
       <c r="F33" s="2">
         <v>41577</v>
       </c>
-      <c r="J33" s="11"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="9"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="9"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="7"/>
-      <c r="Z33" s="9"/>
-      <c r="AB33" s="11"/>
-      <c r="AF33" s="7"/>
-      <c r="AG33" s="9"/>
-      <c r="AI33" s="11"/>
-      <c r="AM33" s="7"/>
-      <c r="AN33" s="9"/>
-      <c r="AO33" s="11"/>
-      <c r="AP33" s="11"/>
+      <c r="I33" t="s">
+        <v>55</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="M33" t="s">
+        <v>59</v>
+      </c>
+      <c r="N33" t="s">
+        <v>59</v>
+      </c>
+      <c r="O33" t="s">
+        <v>59</v>
+      </c>
+      <c r="P33" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>59</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="T33" t="s">
+        <v>59</v>
+      </c>
+      <c r="U33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="V33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="W33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="X33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AL33" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN33" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP33" s="11" t="s">
+        <v>59</v>
+      </c>
       <c r="AQ33" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR33" s="11"/>
+    </row>
+    <row r="34" spans="1:44" customFormat="1">
+      <c r="A34" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="2">
+        <v>41577</v>
+      </c>
+      <c r="F34" s="2">
+        <v>41577</v>
+      </c>
+      <c r="J34" s="11"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="9"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="9"/>
+      <c r="U34" s="11"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="11"/>
+      <c r="X34" s="11"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="9"/>
+      <c r="AB34" s="11"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="9"/>
+      <c r="AI34" s="11"/>
+      <c r="AM34" s="7"/>
+      <c r="AN34" s="9"/>
+      <c r="AO34" s="11"/>
+      <c r="AP34" s="11"/>
+      <c r="AQ34" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AR33" s="11"/>
-    </row>
-    <row r="34" spans="1:44" customFormat="1">
-      <c r="J34" s="11"/>
-    </row>
-    <row r="35" spans="1:44" customFormat="1"/>
+      <c r="AR34" s="11"/>
+    </row>
+    <row r="35" spans="1:44" customFormat="1">
+      <c r="J35" s="11"/>
+    </row>
     <row r="36" spans="1:44" customFormat="1"/>
     <row r="37" spans="1:44" customFormat="1"/>
+    <row r="38" spans="1:44" customFormat="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:AR1"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:AQ33">
+  <conditionalFormatting sqref="J3:AQ34">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Aufgaben technisches Klassenmodell (GUI, Controller und DB-Schicht hinzugefügt)
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16335" windowHeight="6720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19140" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="78">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Design Guide erstellen</t>
   </si>
   <si>
-    <t>Aktivitätsdiagram erstellen</t>
-  </si>
-  <si>
     <t>Logisches DB- Modell erstellen</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>Abstimmung mit Auftraggeber</t>
   </si>
   <si>
-    <t>Abgabe detaillierte Aufwandsschätzung (nach Abstimmung bzgl. Design Guide)</t>
-  </si>
-  <si>
     <t>Beschreibung</t>
   </si>
   <si>
@@ -237,9 +231,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Klassenmodell erstellen</t>
-  </si>
-  <si>
     <t>Datenbank</t>
   </si>
   <si>
@@ -277,6 +268,27 @@
   </si>
   <si>
     <t>Anforderungen und deren Lösungen, inkl. Aufwandsschätzung</t>
+  </si>
+  <si>
+    <t>fachliches Klassenmodell erstellen</t>
+  </si>
+  <si>
+    <t>Rework</t>
+  </si>
+  <si>
+    <t>technisches Klassenmodell - Modelschicht</t>
+  </si>
+  <si>
+    <t>technisches Klassenmodell - Controllerschicht</t>
+  </si>
+  <si>
+    <t>technisches Klassenmodell - GUI-Schicht</t>
+  </si>
+  <si>
+    <t>Review durch TPL Angelos</t>
+  </si>
+  <si>
+    <t>Abgabe Pflichtenheft inkl. detaillierte Aufwandsschätzung</t>
   </si>
 </sst>
 </file>
@@ -384,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -400,6 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -701,15 +714,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR38"/>
+  <dimension ref="A1:AR40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="2" max="2" width="33.75" customWidth="1"/>
+    <col min="2" max="2" width="39.25" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="11.25" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="10.5" customWidth="1" outlineLevel="1"/>
@@ -721,13 +735,13 @@
   <sheetData>
     <row r="1" spans="1:44">
       <c r="J1" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O1" s="12"/>
       <c r="P1" s="12"/>
@@ -762,31 +776,31 @@
     </row>
     <row r="2" spans="1:44">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J2" s="5">
         <v>41544</v>
@@ -896,13 +910,16 @@
     </row>
     <row r="3" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3" s="2">
         <v>41544</v>
@@ -911,13 +928,13 @@
         <v>41544</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K3" s="7"/>
       <c r="L3" s="9"/>
@@ -942,13 +959,16 @@
     </row>
     <row r="4" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
       </c>
       <c r="E4" s="2">
         <v>41544</v>
@@ -957,25 +977,25 @@
         <v>41551</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R4" s="7"/>
       <c r="S4" s="9"/>
@@ -998,13 +1018,13 @@
     </row>
     <row r="5" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
         <v>41544</v>
@@ -1013,31 +1033,31 @@
         <v>41551</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R5" s="7"/>
       <c r="S5" s="9"/>
@@ -1085,30 +1105,36 @@
     </row>
     <row r="7" spans="1:44" customFormat="1">
       <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" s="2">
         <v>41555</v>
       </c>
       <c r="F7" s="2">
         <v>41555</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>44</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="7"/>
       <c r="L7" s="9"/>
       <c r="Q7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="R7" s="7"/>
       <c r="S7" s="9"/>
       <c r="U7" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
@@ -1151,13 +1177,16 @@
     </row>
     <row r="9" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
       </c>
       <c r="E9" s="2">
         <v>41555</v>
@@ -1166,46 +1195,46 @@
         <v>41557</v>
       </c>
       <c r="G9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="7"/>
       <c r="L9" s="9"/>
       <c r="M9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Q9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="T9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="U9" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W9" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X9" s="11"/>
       <c r="Y9" s="7"/>
@@ -1223,13 +1252,13 @@
     </row>
     <row r="10" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2">
         <v>41555</v>
@@ -1237,8 +1266,11 @@
       <c r="F10" s="2">
         <v>41556</v>
       </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="7"/>
@@ -1246,10 +1278,10 @@
       <c r="R10" s="7"/>
       <c r="S10" s="9"/>
       <c r="U10" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W10" s="11"/>
       <c r="X10" s="11"/>
@@ -1268,37 +1300,31 @@
     </row>
     <row r="11" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2">
         <v>41555</v>
       </c>
       <c r="F11" s="2">
-        <v>41557</v>
+        <v>41556</v>
       </c>
       <c r="H11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="7"/>
       <c r="L11" s="9"/>
       <c r="R11" s="7"/>
       <c r="S11" s="9"/>
-      <c r="U11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V11" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="W11" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="U11" s="11"/>
+      <c r="V11" s="11"/>
+      <c r="W11" s="11"/>
       <c r="X11" s="11"/>
       <c r="Y11" s="7"/>
       <c r="Z11" s="9"/>
@@ -1315,37 +1341,31 @@
     </row>
     <row r="12" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E12" s="2">
         <v>41555</v>
       </c>
       <c r="F12" s="2">
-        <v>41557</v>
+        <v>41556</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="J12" s="11"/>
       <c r="K12" s="7"/>
       <c r="L12" s="9"/>
       <c r="R12" s="7"/>
       <c r="S12" s="9"/>
-      <c r="U12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="W12" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="U12" s="11"/>
+      <c r="V12" s="11"/>
+      <c r="W12" s="11"/>
       <c r="X12" s="11"/>
       <c r="Y12" s="7"/>
       <c r="Z12" s="9"/>
@@ -1362,35 +1382,39 @@
     </row>
     <row r="13" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2">
-        <v>41557</v>
+        <v>41555</v>
       </c>
       <c r="F13" s="2">
         <v>41557</v>
       </c>
+      <c r="G13" t="s">
+        <v>47</v>
+      </c>
       <c r="H13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="7"/>
       <c r="L13" s="9"/>
       <c r="R13" s="7"/>
       <c r="S13" s="9"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
+      <c r="U13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="V13" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="W13" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X13" s="11"/>
       <c r="Y13" s="7"/>
@@ -1406,15 +1430,39 @@
       <c r="AQ13" s="11"/>
       <c r="AR13" s="11"/>
     </row>
-    <row r="14" spans="1:44" customFormat="1">
+    <row r="14" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="2">
+        <v>41555</v>
+      </c>
+      <c r="F14" s="2">
+        <v>41557</v>
+      </c>
+      <c r="H14" t="s">
+        <v>39</v>
+      </c>
       <c r="J14" s="11"/>
       <c r="K14" s="7"/>
       <c r="L14" s="9"/>
       <c r="R14" s="7"/>
       <c r="S14" s="9"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
+      <c r="U14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="V14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="W14" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="X14" s="11"/>
       <c r="Y14" s="7"/>
       <c r="Z14" s="9"/>
@@ -1429,21 +1477,27 @@
       <c r="AQ14" s="11"/>
       <c r="AR14" s="11"/>
     </row>
-    <row r="15" spans="1:44" customFormat="1">
+    <row r="15" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2">
         <v>41557</v>
       </c>
       <c r="F15" s="2">
         <v>41557</v>
+      </c>
+      <c r="H15" t="s">
+        <v>69</v>
+      </c>
+      <c r="I15" t="s">
+        <v>70</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="7"/>
@@ -1453,7 +1507,7 @@
       <c r="U15" s="11"/>
       <c r="V15" s="11"/>
       <c r="W15" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="X15" s="11"/>
       <c r="Y15" s="7"/>
@@ -1470,24 +1524,6 @@
       <c r="AR15" s="11"/>
     </row>
     <row r="16" spans="1:44" customFormat="1">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" s="2">
-        <v>41557</v>
-      </c>
-      <c r="F16" s="2">
-        <v>41557</v>
-      </c>
-      <c r="H16" t="s">
-        <v>47</v>
-      </c>
       <c r="J16" s="11"/>
       <c r="K16" s="7"/>
       <c r="L16" s="9"/>
@@ -1495,9 +1531,7 @@
       <c r="S16" s="9"/>
       <c r="U16" s="11"/>
       <c r="V16" s="11"/>
-      <c r="W16" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="W16" s="11"/>
       <c r="X16" s="11"/>
       <c r="Y16" s="7"/>
       <c r="Z16" s="9"/>
@@ -1513,6 +1547,24 @@
       <c r="AR16" s="11"/>
     </row>
     <row r="17" spans="1:44" customFormat="1">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="2">
+        <v>41557</v>
+      </c>
+      <c r="F17" s="2">
+        <v>41557</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
       <c r="J17" s="11"/>
       <c r="K17" s="7"/>
       <c r="L17" s="9"/>
@@ -1520,7 +1572,9 @@
       <c r="S17" s="9"/>
       <c r="U17" s="11"/>
       <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
+      <c r="W17" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="X17" s="11"/>
       <c r="Y17" s="7"/>
       <c r="Z17" s="9"/>
@@ -1535,25 +1589,7 @@
       <c r="AQ17" s="11"/>
       <c r="AR17" s="11"/>
     </row>
-    <row r="18" spans="1:44" customFormat="1" outlineLevel="1">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2">
-        <v>41557</v>
-      </c>
-      <c r="F18" s="2">
-        <v>41557</v>
-      </c>
-      <c r="H18" t="s">
-        <v>41</v>
-      </c>
+    <row r="18" spans="1:44" customFormat="1">
       <c r="J18" s="11"/>
       <c r="K18" s="7"/>
       <c r="L18" s="9"/>
@@ -1561,9 +1597,7 @@
       <c r="S18" s="9"/>
       <c r="U18" s="11"/>
       <c r="V18" s="11"/>
-      <c r="W18" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="W18" s="11"/>
       <c r="X18" s="11"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="9"/>
@@ -1580,19 +1614,22 @@
     </row>
     <row r="19" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2">
         <v>41557</v>
       </c>
       <c r="F19" s="2">
-        <v>41562</v>
+        <v>41557</v>
+      </c>
+      <c r="H19" t="s">
+        <v>40</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="7"/>
@@ -1602,23 +1639,12 @@
       <c r="U19" s="11"/>
       <c r="V19" s="11"/>
       <c r="W19" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X19" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y19" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z19" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA19" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB19" s="11" t="s">
-        <v>59</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="9"/>
+      <c r="AB19" s="11"/>
       <c r="AF19" s="7"/>
       <c r="AG19" s="9"/>
       <c r="AI19" s="11"/>
@@ -1631,13 +1657,13 @@
     </row>
     <row r="20" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2">
         <v>41557</v>
@@ -1653,22 +1679,22 @@
       <c r="U20" s="11"/>
       <c r="V20" s="11"/>
       <c r="W20" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X20" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y20" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z20" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AA20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB20" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AF20" s="7"/>
       <c r="AG20" s="9"/>
@@ -1682,13 +1708,13 @@
     </row>
     <row r="21" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2">
         <v>41557</v>
@@ -1704,22 +1730,22 @@
       <c r="U21" s="11"/>
       <c r="V21" s="11"/>
       <c r="W21" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X21" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y21" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z21" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AA21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB21" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AF21" s="7"/>
       <c r="AG21" s="9"/>
@@ -1733,13 +1759,13 @@
     </row>
     <row r="22" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2">
         <v>41557</v>
@@ -1755,22 +1781,22 @@
       <c r="U22" s="11"/>
       <c r="V22" s="11"/>
       <c r="W22" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X22" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y22" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z22" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AA22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB22" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AF22" s="7"/>
       <c r="AG22" s="9"/>
@@ -1784,10 +1810,10 @@
     </row>
     <row r="23" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1806,22 +1832,22 @@
       <c r="U23" s="11"/>
       <c r="V23" s="11"/>
       <c r="W23" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X23" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y23" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z23" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AA23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB23" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AF23" s="7"/>
       <c r="AG23" s="9"/>
@@ -1835,13 +1861,13 @@
     </row>
     <row r="24" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2">
         <v>41557</v>
@@ -1857,22 +1883,22 @@
       <c r="U24" s="11"/>
       <c r="V24" s="11"/>
       <c r="W24" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="X24" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Y24" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="Z24" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AA24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB24" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AF24" s="7"/>
       <c r="AG24" s="9"/>
@@ -1886,16 +1912,16 @@
     </row>
     <row r="25" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E25" s="2">
-        <v>41562</v>
+        <v>41557</v>
       </c>
       <c r="F25" s="2">
         <v>41562</v>
@@ -1907,12 +1933,23 @@
       <c r="S25" s="9"/>
       <c r="U25" s="11"/>
       <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="7"/>
-      <c r="Z25" s="9"/>
+      <c r="W25" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="X25" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z25" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>57</v>
+      </c>
       <c r="AB25" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF25" s="7"/>
       <c r="AG25" s="9"/>
@@ -1926,19 +1963,19 @@
     </row>
     <row r="26" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E26" s="2">
         <v>41562</v>
       </c>
       <c r="F26" s="2">
-        <v>41569</v>
+        <v>41562</v>
       </c>
       <c r="J26" s="11"/>
       <c r="K26" s="7"/>
@@ -1952,23 +1989,10 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="9"/>
       <c r="AB26" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC26" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE26" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF26" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG26" s="9" t="s">
-        <v>59</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="AF26" s="7"/>
+      <c r="AG26" s="9"/>
       <c r="AI26" s="11"/>
       <c r="AM26" s="7"/>
       <c r="AN26" s="9"/>
@@ -1977,7 +2001,22 @@
       <c r="AQ26" s="11"/>
       <c r="AR26" s="11"/>
     </row>
-    <row r="27" spans="1:44" customFormat="1">
+    <row r="27" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="2">
+        <v>41562</v>
+      </c>
+      <c r="F27" s="2">
+        <v>41569</v>
+      </c>
       <c r="J27" s="11"/>
       <c r="K27" s="7"/>
       <c r="L27" s="9"/>
@@ -1989,9 +2028,24 @@
       <c r="X27" s="11"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="9"/>
-      <c r="AB27" s="11"/>
-      <c r="AF27" s="7"/>
-      <c r="AG27" s="9"/>
+      <c r="AB27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF27" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG27" s="9" t="s">
+        <v>57</v>
+      </c>
       <c r="AI27" s="11"/>
       <c r="AM27" s="7"/>
       <c r="AN27" s="9"/>
@@ -2000,22 +2054,7 @@
       <c r="AQ27" s="11"/>
       <c r="AR27" s="11"/>
     </row>
-    <row r="28" spans="1:44" customFormat="1" outlineLevel="1">
-      <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E28" s="2">
-        <v>41562</v>
-      </c>
-      <c r="F28" s="2">
-        <v>41577</v>
-      </c>
+    <row r="28" spans="1:44" customFormat="1">
       <c r="J28" s="11"/>
       <c r="K28" s="7"/>
       <c r="L28" s="9"/>
@@ -2027,65 +2066,26 @@
       <c r="X28" s="11"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="9"/>
-      <c r="AB28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL28" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM28" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP28" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ28" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="AB28" s="11"/>
+      <c r="AF28" s="7"/>
+      <c r="AG28" s="9"/>
+      <c r="AI28" s="11"/>
+      <c r="AM28" s="7"/>
+      <c r="AN28" s="9"/>
+      <c r="AO28" s="11"/>
+      <c r="AP28" s="11"/>
+      <c r="AQ28" s="11"/>
       <c r="AR28" s="11"/>
     </row>
     <row r="29" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
         <v>31</v>
       </c>
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="2">
         <v>41562</v>
@@ -2105,67 +2105,67 @@
       <c r="Y29" s="7"/>
       <c r="Z29" s="9"/>
       <c r="AB29" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AC29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AD29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AE29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AF29" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AG29" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AH29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AI29" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AJ29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AK29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AL29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AM29" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AN29" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AO29" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AP29" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AQ29" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AR29" s="11"/>
     </row>
     <row r="30" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E30" s="2">
-        <v>41577</v>
+        <v>41562</v>
       </c>
       <c r="F30" s="2">
         <v>41577</v>
@@ -2181,31 +2181,68 @@
       <c r="X30" s="11"/>
       <c r="Y30" s="7"/>
       <c r="Z30" s="9"/>
-      <c r="AB30" s="11"/>
-      <c r="AF30" s="7"/>
-      <c r="AG30" s="9"/>
-      <c r="AI30" s="11"/>
-      <c r="AM30" s="7"/>
-      <c r="AN30" s="9"/>
-      <c r="AO30" s="11"/>
-      <c r="AP30" s="11"/>
+      <c r="AB30" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI30" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL30" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO30" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP30" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="AQ30" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AR30" s="11"/>
     </row>
     <row r="31" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E31" s="2">
-        <v>41562</v>
+        <v>41577</v>
       </c>
       <c r="F31" s="2">
         <v>41577</v>
@@ -2221,59 +2258,35 @@
       <c r="X31" s="11"/>
       <c r="Y31" s="7"/>
       <c r="Z31" s="9"/>
-      <c r="AB31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF31" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG31" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL31" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM31" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN31" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP31" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="AB31" s="11"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="9"/>
+      <c r="AI31" s="11"/>
+      <c r="AM31" s="7"/>
+      <c r="AN31" s="9"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="11"/>
       <c r="AQ31" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AR31" s="11"/>
     </row>
-    <row r="32" spans="1:44" customFormat="1">
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+    <row r="32" spans="1:44" customFormat="1" outlineLevel="1">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="2">
+        <v>41562</v>
+      </c>
+      <c r="F32" s="2">
+        <v>41577</v>
+      </c>
       <c r="J32" s="11"/>
       <c r="K32" s="7"/>
       <c r="L32" s="9"/>
@@ -2285,192 +2298,257 @@
       <c r="X32" s="11"/>
       <c r="Y32" s="7"/>
       <c r="Z32" s="9"/>
-      <c r="AB32" s="11"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="9"/>
-      <c r="AI32" s="11"/>
-      <c r="AM32" s="7"/>
-      <c r="AN32" s="9"/>
-      <c r="AO32" s="11"/>
-      <c r="AP32" s="11"/>
-      <c r="AQ32" s="11"/>
+      <c r="AB32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL32" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM32" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ32" s="11" t="s">
+        <v>56</v>
+      </c>
       <c r="AR32" s="11"/>
     </row>
     <row r="33" spans="1:44" customFormat="1">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
-      <c r="B33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" s="2">
-        <v>41544</v>
-      </c>
-      <c r="F33" s="2">
-        <v>41577</v>
-      </c>
-      <c r="I33" t="s">
-        <v>55</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="K33" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="L33" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M33" t="s">
-        <v>59</v>
-      </c>
-      <c r="N33" t="s">
-        <v>59</v>
-      </c>
-      <c r="O33" t="s">
-        <v>59</v>
-      </c>
-      <c r="P33" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>59</v>
-      </c>
-      <c r="R33" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="S33" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="T33" t="s">
-        <v>59</v>
-      </c>
-      <c r="U33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="V33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="W33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="X33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y33" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z33" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AE33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF33" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG33" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AK33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL33" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM33" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AN33" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AP33" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="AQ33" s="11" t="s">
-        <v>59</v>
-      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="9"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="9"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+      <c r="W33" s="11"/>
+      <c r="X33" s="11"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="9"/>
+      <c r="AB33" s="11"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="9"/>
+      <c r="AI33" s="11"/>
+      <c r="AM33" s="7"/>
+      <c r="AN33" s="9"/>
+      <c r="AO33" s="11"/>
+      <c r="AP33" s="11"/>
+      <c r="AQ33" s="11"/>
       <c r="AR33" s="11"/>
     </row>
     <row r="34" spans="1:44" customFormat="1">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="E34" s="2">
-        <v>41577</v>
+        <v>41544</v>
       </c>
       <c r="F34" s="2">
         <v>41577</v>
       </c>
-      <c r="J34" s="11"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="9"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="9"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="7"/>
-      <c r="Z34" s="9"/>
-      <c r="AB34" s="11"/>
-      <c r="AF34" s="7"/>
-      <c r="AG34" s="9"/>
-      <c r="AI34" s="11"/>
-      <c r="AM34" s="7"/>
-      <c r="AN34" s="9"/>
-      <c r="AO34" s="11"/>
-      <c r="AP34" s="11"/>
+      <c r="I34" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M34" t="s">
+        <v>57</v>
+      </c>
+      <c r="N34" t="s">
+        <v>57</v>
+      </c>
+      <c r="O34" t="s">
+        <v>57</v>
+      </c>
+      <c r="P34" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>57</v>
+      </c>
+      <c r="R34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="T34" t="s">
+        <v>57</v>
+      </c>
+      <c r="U34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="V34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="W34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="X34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL34" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP34" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="AQ34" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AR34" s="11"/>
     </row>
     <row r="35" spans="1:44" customFormat="1">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="2">
+        <v>41577</v>
+      </c>
+      <c r="F35" s="2">
+        <v>41577</v>
+      </c>
       <c r="J35" s="11"/>
-    </row>
-    <row r="36" spans="1:44" customFormat="1"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="9"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="9"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="9"/>
+      <c r="AB35" s="11"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="9"/>
+      <c r="AI35" s="11"/>
+      <c r="AM35" s="7"/>
+      <c r="AN35" s="9"/>
+      <c r="AO35" s="11"/>
+      <c r="AP35" s="11"/>
+      <c r="AQ35" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR35" s="11"/>
+    </row>
+    <row r="36" spans="1:44" customFormat="1">
+      <c r="J36" s="11"/>
+    </row>
     <row r="37" spans="1:44" customFormat="1"/>
     <row r="38" spans="1:44" customFormat="1"/>
+    <row r="39" spans="1:44" customFormat="1"/>
+    <row r="40" spans="1:44" customFormat="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:AR1"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:AQ34">
+  <conditionalFormatting sqref="J3:AQ35">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
@@ -2501,57 +2579,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aktuallisiert (Zuorndung Test-> Ralf)
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="71">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Angelos</t>
   </si>
   <si>
-    <t>offen</t>
-  </si>
-  <si>
     <t>DB erstellen</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
   </si>
   <si>
     <t>Installer erstellen</t>
-  </si>
-  <si>
-    <t>Lasttest</t>
   </si>
   <si>
     <t>Testdokumentation</t>
@@ -690,8 +684,8 @@
   <dimension ref="A1:AR41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
+      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -707,13 +701,13 @@
   <sheetData>
     <row r="1" spans="1:44">
       <c r="I1" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
@@ -748,7 +742,7 @@
     </row>
     <row r="2" spans="1:44">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -757,19 +751,19 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I2" s="4">
         <v>41544</v>
@@ -879,7 +873,7 @@
     </row>
     <row r="3" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -897,13 +891,13 @@
         <v>41544</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="8"/>
@@ -928,10 +922,10 @@
     </row>
     <row r="4" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -946,43 +940,43 @@
         <v>41554</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
@@ -1003,10 +997,10 @@
     </row>
     <row r="5" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -1021,43 +1015,43 @@
         <v>41554</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
@@ -1078,7 +1072,7 @@
     </row>
     <row r="6" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -1093,43 +1087,43 @@
         <v>41554</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="P6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
@@ -1175,13 +1169,13 @@
     </row>
     <row r="8" spans="1:44" customFormat="1">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -1193,7 +1187,7 @@
         <v>41555</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="6"/>
@@ -1201,7 +1195,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="8"/>
       <c r="T8" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
@@ -1244,7 +1238,7 @@
     </row>
     <row r="10" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1262,10 +1256,10 @@
         <v>41557</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I10" s="10"/>
       <c r="J10" s="6"/>
@@ -1273,13 +1267,13 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="8"/>
       <c r="T10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V10" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W10" s="10"/>
       <c r="X10" s="6"/>
@@ -1297,10 +1291,10 @@
     </row>
     <row r="11" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1312,10 +1306,10 @@
         <v>41556</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="6"/>
@@ -1323,10 +1317,10 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="8"/>
       <c r="T11" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
@@ -1345,10 +1339,10 @@
     </row>
     <row r="12" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -1360,10 +1354,10 @@
         <v>41556</v>
       </c>
       <c r="G12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I12" s="10"/>
       <c r="J12" s="6"/>
@@ -1389,7 +1383,7 @@
     </row>
     <row r="13" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -1404,10 +1398,10 @@
         <v>41557</v>
       </c>
       <c r="G13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="6"/>
@@ -1415,13 +1409,13 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="8"/>
       <c r="T13" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V13" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W13" s="10"/>
       <c r="X13" s="6"/>
@@ -1439,7 +1433,7 @@
     </row>
     <row r="14" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1454,7 +1448,7 @@
         <v>41557</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="6"/>
@@ -1462,13 +1456,13 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="8"/>
       <c r="T14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="V14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W14" s="10"/>
       <c r="X14" s="6"/>
@@ -1486,13 +1480,13 @@
     </row>
     <row r="15" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E15" s="2">
         <v>41557</v>
@@ -1501,7 +1495,7 @@
         <v>41557</v>
       </c>
       <c r="H15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I15" s="10"/>
       <c r="J15" s="6"/>
@@ -1511,7 +1505,7 @@
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="W15" s="10"/>
       <c r="X15" s="6"/>
@@ -1552,13 +1546,13 @@
     </row>
     <row r="17" spans="1:44" customFormat="1">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" s="2">
         <v>41557</v>
@@ -1567,7 +1561,7 @@
         <v>41557</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="6"/>
@@ -1577,7 +1571,7 @@
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="W17" s="10"/>
       <c r="X17" s="6"/>
@@ -1618,10 +1612,10 @@
     </row>
     <row r="19" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1633,7 +1627,7 @@
         <v>41557</v>
       </c>
       <c r="H19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I19" s="10"/>
       <c r="J19" s="6"/>
@@ -1643,7 +1637,7 @@
       <c r="T19" s="10"/>
       <c r="U19" s="10"/>
       <c r="V19" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W19" s="10"/>
       <c r="X19" s="6"/>
@@ -1661,10 +1655,10 @@
     </row>
     <row r="20" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1683,22 +1677,22 @@
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
       <c r="V20" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W20" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X20" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y20" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA20" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE20" s="6"/>
       <c r="AF20" s="8"/>
@@ -1712,10 +1706,10 @@
     </row>
     <row r="21" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>11</v>
@@ -1734,22 +1728,22 @@
       <c r="T21" s="10"/>
       <c r="U21" s="10"/>
       <c r="V21" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W21" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X21" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y21" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA21" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE21" s="6"/>
       <c r="AF21" s="8"/>
@@ -1763,10 +1757,10 @@
     </row>
     <row r="22" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1785,22 +1779,22 @@
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
       <c r="V22" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W22" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X22" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y22" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA22" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE22" s="6"/>
       <c r="AF22" s="8"/>
@@ -1814,13 +1808,13 @@
     </row>
     <row r="23" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E23" s="2">
         <v>41557</v>
@@ -1836,22 +1830,22 @@
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
       <c r="V23" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W23" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X23" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y23" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA23" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE23" s="6"/>
       <c r="AF23" s="8"/>
@@ -1865,10 +1859,10 @@
     </row>
     <row r="24" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
         <v>11</v>
@@ -1887,22 +1881,22 @@
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
       <c r="V24" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W24" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X24" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y24" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA24" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE24" s="6"/>
       <c r="AF24" s="8"/>
@@ -1916,10 +1910,10 @@
     </row>
     <row r="25" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
         <v>11</v>
@@ -1938,22 +1932,22 @@
       <c r="T25" s="10"/>
       <c r="U25" s="10"/>
       <c r="V25" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W25" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="X25" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Y25" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AA25" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE25" s="6"/>
       <c r="AF25" s="8"/>
@@ -1967,10 +1961,10 @@
     </row>
     <row r="26" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
         <v>11</v>
@@ -1993,7 +1987,7 @@
       <c r="X26" s="6"/>
       <c r="Y26" s="8"/>
       <c r="AA26" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="AE26" s="6"/>
       <c r="AF26" s="8"/>
@@ -2007,13 +2001,13 @@
     </row>
     <row r="27" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="E27" s="2">
         <v>41562</v>
@@ -2033,22 +2027,22 @@
       <c r="X27" s="6"/>
       <c r="Y27" s="8"/>
       <c r="AA27" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AC27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AD27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE27" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AF27" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH27" s="10"/>
       <c r="AL27" s="6"/>
@@ -2083,13 +2077,13 @@
     </row>
     <row r="29" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E29" s="2">
         <v>41562</v>
@@ -2109,64 +2103,64 @@
       <c r="X29" s="6"/>
       <c r="Y29" s="8"/>
       <c r="AA29" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AC29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AD29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE29" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AF29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AG29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH29" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AI29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AJ29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AK29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL29" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AN29" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AO29" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AP29" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ29" s="10"/>
     </row>
     <row r="30" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E30" s="2">
         <v>41562</v>
@@ -2186,67 +2180,67 @@
       <c r="X30" s="6"/>
       <c r="Y30" s="8"/>
       <c r="AA30" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AB30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AC30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AD30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AE30" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AF30" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AG30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AH30" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AI30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AJ30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AK30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AL30" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AM30" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AN30" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AO30" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AP30" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AQ30" s="10"/>
     </row>
     <row r="31" spans="1:44" customFormat="1" outlineLevel="1">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E31" s="2">
-        <v>41577</v>
+        <v>41562</v>
       </c>
       <c r="F31" s="2">
         <v>41577</v>
@@ -2262,35 +2256,59 @@
       <c r="W31" s="10"/>
       <c r="X31" s="6"/>
       <c r="Y31" s="8"/>
-      <c r="AA31" s="10"/>
-      <c r="AE31" s="6"/>
-      <c r="AF31" s="8"/>
-      <c r="AH31" s="10"/>
-      <c r="AL31" s="6"/>
-      <c r="AM31" s="8"/>
-      <c r="AN31" s="10"/>
-      <c r="AO31" s="10"/>
+      <c r="AA31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN31" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO31" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="AP31" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AQ31" s="10"/>
     </row>
-    <row r="32" spans="1:44" customFormat="1" outlineLevel="1">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>23</v>
-      </c>
-      <c r="C32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="2">
-        <v>41562</v>
-      </c>
-      <c r="F32" s="2">
-        <v>41577</v>
-      </c>
+    <row r="32" spans="1:44" customFormat="1">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
       <c r="I32" s="10"/>
       <c r="J32" s="6"/>
       <c r="K32" s="8"/>
@@ -2302,244 +2320,181 @@
       <c r="W32" s="10"/>
       <c r="X32" s="6"/>
       <c r="Y32" s="8"/>
-      <c r="AA32" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF32" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH32" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM32" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN32" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO32" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AP32" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="AA32" s="10"/>
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="8"/>
+      <c r="AH32" s="10"/>
+      <c r="AL32" s="6"/>
+      <c r="AM32" s="8"/>
+      <c r="AN32" s="10"/>
+      <c r="AO32" s="10"/>
+      <c r="AP32" s="10"/>
       <c r="AQ32" s="10"/>
     </row>
     <row r="33" spans="1:44" customFormat="1">
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="8"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="8"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="6"/>
-      <c r="Y33" s="8"/>
-      <c r="AA33" s="10"/>
-      <c r="AE33" s="6"/>
-      <c r="AF33" s="8"/>
-      <c r="AH33" s="10"/>
-      <c r="AL33" s="6"/>
-      <c r="AM33" s="8"/>
-      <c r="AN33" s="10"/>
-      <c r="AO33" s="10"/>
-      <c r="AP33" s="10"/>
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="2">
+        <v>41544</v>
+      </c>
+      <c r="F33" s="2">
+        <v>41577</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L33" t="s">
+        <v>52</v>
+      </c>
+      <c r="M33" t="s">
+        <v>52</v>
+      </c>
+      <c r="N33" t="s">
+        <v>52</v>
+      </c>
+      <c r="O33" t="s">
+        <v>52</v>
+      </c>
+      <c r="P33" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="R33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="S33" t="s">
+        <v>52</v>
+      </c>
+      <c r="T33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="U33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="V33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="W33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="X33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK33" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL33" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP33" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="AQ33" s="10"/>
     </row>
     <row r="34" spans="1:44" customFormat="1">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E34" s="2">
-        <v>41544</v>
+        <v>41577</v>
       </c>
       <c r="F34" s="2">
         <v>41577</v>
       </c>
-      <c r="I34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K34" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="L34" t="s">
-        <v>54</v>
-      </c>
-      <c r="M34" t="s">
-        <v>54</v>
-      </c>
-      <c r="N34" t="s">
-        <v>54</v>
-      </c>
-      <c r="O34" t="s">
-        <v>54</v>
-      </c>
-      <c r="P34" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="R34" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="S34" t="s">
-        <v>54</v>
-      </c>
-      <c r="T34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="U34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="V34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="W34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="X34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y34" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AC34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AF34" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK34" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL34" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM34" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="AO34" s="10" t="s">
-        <v>54</v>
-      </c>
+      <c r="I34" s="10"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="8"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="8"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+      <c r="W34" s="10"/>
+      <c r="X34" s="6"/>
+      <c r="Y34" s="8"/>
+      <c r="AA34" s="10"/>
+      <c r="AE34" s="6"/>
+      <c r="AF34" s="8"/>
+      <c r="AH34" s="10"/>
+      <c r="AL34" s="6"/>
+      <c r="AM34" s="8"/>
+      <c r="AN34" s="10"/>
+      <c r="AO34" s="10"/>
       <c r="AP34" s="10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AQ34" s="10"/>
     </row>
     <row r="35" spans="1:44" customFormat="1">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="2">
-        <v>41577</v>
-      </c>
-      <c r="F35" s="2">
-        <v>41577</v>
-      </c>
       <c r="I35" s="10"/>
-      <c r="J35" s="6"/>
-      <c r="K35" s="8"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="8"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="10"/>
-      <c r="X35" s="6"/>
-      <c r="Y35" s="8"/>
-      <c r="AA35" s="10"/>
-      <c r="AE35" s="6"/>
-      <c r="AF35" s="8"/>
-      <c r="AH35" s="10"/>
-      <c r="AL35" s="6"/>
-      <c r="AM35" s="8"/>
-      <c r="AN35" s="10"/>
-      <c r="AO35" s="10"/>
-      <c r="AP35" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ35" s="10"/>
-    </row>
-    <row r="36" spans="1:44" customFormat="1">
-      <c r="I36" s="10"/>
-    </row>
+    </row>
+    <row r="36" spans="1:44" customFormat="1"/>
     <row r="37" spans="1:44" customFormat="1"/>
     <row r="38" spans="1:44" customFormat="1"/>
     <row r="39" spans="1:44" customFormat="1"/>
@@ -2550,7 +2505,7 @@
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:AQ1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:AP35">
+  <conditionalFormatting sqref="I3:AP34">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
@@ -2581,57 +2536,57 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gesamtaufwand und Hinterlegung Status Aufgaben
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
     <sheet name="Teams" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="73">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -272,6 +272,12 @@
   </si>
   <si>
     <t>Anforderungskatalog erstellen</t>
+  </si>
+  <si>
+    <t>Aufwand gesamt</t>
+  </si>
+  <si>
+    <t>Aufwand p.P.</t>
   </si>
 </sst>
 </file>
@@ -368,7 +374,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -384,11 +390,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -688,23 +835,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ35"/>
+  <dimension ref="A1:AQ37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AR15" sqref="AR15"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.25" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.25" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="10.375" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="11.625" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="8" max="8" width="39.75" hidden="1" customWidth="1" outlineLevel="2"/>
-    <col min="9" max="9" width="3.125" customWidth="1" collapsed="1"/>
-    <col min="10" max="43" width="3.125" customWidth="1"/>
+    <col min="4" max="5" width="11.25" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="10.375" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1" outlineLevel="2"/>
+    <col min="8" max="8" width="39.75" customWidth="1" outlineLevel="2"/>
+    <col min="9" max="43" width="3.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.2">
@@ -1471,6 +1617,9 @@
       <c r="F14" s="2">
         <v>41557</v>
       </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
       <c r="H14" t="s">
         <v>36</v>
       </c>
@@ -1517,6 +1666,9 @@
       </c>
       <c r="F15" s="2">
         <v>41557</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
       </c>
       <c r="H15" t="s">
         <v>63</v>
@@ -2525,19 +2677,68 @@
       <c r="AQ34" s="10"/>
     </row>
     <row r="35" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
       <c r="I35" s="10"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="8"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="8"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="8"/>
+      <c r="AA35" s="10"/>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="8"/>
+      <c r="AH35" s="10"/>
+      <c r="AL35" s="6"/>
+      <c r="AM35" s="8"/>
+      <c r="AN35" s="10"/>
+      <c r="AO35" s="10"/>
+      <c r="AP35" s="10"/>
+      <c r="AQ35" s="10"/>
+    </row>
+    <row r="36" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36">
+        <f>SUM(D6:D34)</f>
+        <v>168</v>
+      </c>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="13">
+        <f>D36/11</f>
+        <v>15.272727272727273</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:AQ1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:AP34">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="I3:AP35">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"x"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"m"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:G34">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"m"</formula>
+      <formula>"erledigt"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REWORK Philipp aktualisiert auf ERLEDIGT (Y)
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Fallstudie\Projektmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phil\git\Fallstudie\Projektmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -266,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -698,22 +698,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.25" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.25" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="11.75" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="11.625" customWidth="1" outlineLevel="2"/>
-    <col min="8" max="42" width="3.125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1" outlineLevel="2"/>
+    <col min="8" max="42" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="H1" s="13" t="s">
         <v>40</v>
       </c>
@@ -754,7 +754,7 @@
       <c r="AO1" s="13"/>
       <c r="AP1" s="13"/>
     </row>
-    <row r="2" spans="1:42">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
@@ -882,7 +882,7 @@
         <v>41578</v>
       </c>
     </row>
-    <row r="3" spans="1:42" outlineLevel="1">
+    <row r="3" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -928,7 +928,7 @@
       <c r="AO3" s="10"/>
       <c r="AP3" s="10"/>
     </row>
-    <row r="4" spans="1:42" outlineLevel="1">
+    <row r="4" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1000,7 +1000,7 @@
       <c r="AO4" s="10"/>
       <c r="AP4" s="10"/>
     </row>
-    <row r="5" spans="1:42" outlineLevel="1">
+    <row r="5" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="AO5" s="10"/>
       <c r="AP5" s="10"/>
     </row>
-    <row r="6" spans="1:42" outlineLevel="1">
+    <row r="6" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1144,7 +1144,7 @@
       <c r="AO6" s="10"/>
       <c r="AP6" s="10"/>
     </row>
-    <row r="7" spans="1:42">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="H7" s="10"/>
@@ -1169,7 +1169,7 @@
       <c r="AO7" s="10"/>
       <c r="AP7" s="10"/>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1215,7 +1215,7 @@
       <c r="AO8" s="10"/>
       <c r="AP8" s="10"/>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="H9" s="10"/>
       <c r="I9" s="6"/>
       <c r="J9" s="8"/>
@@ -1238,7 +1238,7 @@
       <c r="AO9" s="10"/>
       <c r="AP9" s="10"/>
     </row>
-    <row r="10" spans="1:42" outlineLevel="1">
+    <row r="10" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1288,7 +1288,7 @@
       <c r="AO10" s="10"/>
       <c r="AP10" s="10"/>
     </row>
-    <row r="11" spans="1:42" outlineLevel="1">
+    <row r="11" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1308,7 +1308,7 @@
         <v>41556</v>
       </c>
       <c r="G11" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="6"/>
@@ -1336,7 +1336,7 @@
       <c r="AO11" s="10"/>
       <c r="AP11" s="10"/>
     </row>
-    <row r="12" spans="1:42" outlineLevel="1">
+    <row r="12" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1384,7 +1384,7 @@
       <c r="AO12" s="10"/>
       <c r="AP12" s="10"/>
     </row>
-    <row r="13" spans="1:42" outlineLevel="1">
+    <row r="13" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="AO13" s="10"/>
       <c r="AP13" s="10"/>
     </row>
-    <row r="14" spans="1:42" outlineLevel="1">
+    <row r="14" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1484,7 +1484,7 @@
       <c r="AO14" s="10"/>
       <c r="AP14" s="10"/>
     </row>
-    <row r="15" spans="1:42" outlineLevel="1">
+    <row r="15" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1534,7 +1534,7 @@
       <c r="AO15" s="10"/>
       <c r="AP15" s="10"/>
     </row>
-    <row r="16" spans="1:42" outlineLevel="1">
+    <row r="16" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="AO16" s="10"/>
       <c r="AP16" s="10"/>
     </row>
-    <row r="17" spans="1:42">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="H17" s="10"/>
       <c r="I17" s="6"/>
       <c r="J17" s="8"/>
@@ -1603,7 +1603,7 @@
       <c r="AO17" s="10"/>
       <c r="AP17" s="10"/>
     </row>
-    <row r="18" spans="1:42">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="AO18" s="10"/>
       <c r="AP18" s="10"/>
     </row>
-    <row r="19" spans="1:42">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="H19" s="10"/>
       <c r="I19" s="6"/>
       <c r="J19" s="8"/>
@@ -1672,7 +1672,7 @@
       <c r="AO19" s="10"/>
       <c r="AP19" s="10"/>
     </row>
-    <row r="20" spans="1:42" outlineLevel="1">
+    <row r="20" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1715,7 +1715,7 @@
       <c r="AO20" s="10"/>
       <c r="AP20" s="10"/>
     </row>
-    <row r="21" spans="1:42" outlineLevel="1">
+    <row r="21" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="AO21" s="10"/>
       <c r="AP21" s="10"/>
     </row>
-    <row r="22" spans="1:42" outlineLevel="1">
+    <row r="22" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1823,7 +1823,7 @@
       <c r="AO22" s="10"/>
       <c r="AP22" s="10"/>
     </row>
-    <row r="23" spans="1:42" outlineLevel="1">
+    <row r="23" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -1877,7 +1877,7 @@
       <c r="AO23" s="10"/>
       <c r="AP23" s="10"/>
     </row>
-    <row r="24" spans="1:42" outlineLevel="1">
+    <row r="24" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1931,7 +1931,7 @@
       <c r="AO24" s="10"/>
       <c r="AP24" s="10"/>
     </row>
-    <row r="25" spans="1:42" outlineLevel="1">
+    <row r="25" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1985,7 +1985,7 @@
       <c r="AO25" s="10"/>
       <c r="AP25" s="10"/>
     </row>
-    <row r="26" spans="1:42" outlineLevel="1">
+    <row r="26" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="AO26" s="10"/>
       <c r="AP26" s="10"/>
     </row>
-    <row r="27" spans="1:42" outlineLevel="1">
+    <row r="27" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="AO27" s="10"/>
       <c r="AP27" s="10"/>
     </row>
-    <row r="28" spans="1:42" outlineLevel="1">
+    <row r="28" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="AO28" s="10"/>
       <c r="AP28" s="10"/>
     </row>
-    <row r="29" spans="1:42">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="H29" s="10"/>
       <c r="I29" s="6"/>
       <c r="J29" s="8"/>
@@ -2157,7 +2157,7 @@
       <c r="AO29" s="10"/>
       <c r="AP29" s="10"/>
     </row>
-    <row r="30" spans="1:42" outlineLevel="1">
+    <row r="30" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="AP30" s="10"/>
     </row>
-    <row r="31" spans="1:42" outlineLevel="1">
+    <row r="31" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="AP31" s="10"/>
     </row>
-    <row r="32" spans="1:42" outlineLevel="1">
+    <row r="32" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="AP32" s="10"/>
     </row>
-    <row r="33" spans="1:42" outlineLevel="1">
+    <row r="33" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -2437,7 +2437,7 @@
       <c r="AO33" s="10"/>
       <c r="AP33" s="10"/>
     </row>
-    <row r="34" spans="1:42" outlineLevel="1">
+    <row r="34" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>27</v>
       </c>
@@ -2477,7 +2477,7 @@
       <c r="AO34" s="10"/>
       <c r="AP34" s="10"/>
     </row>
-    <row r="35" spans="1:42" outlineLevel="1">
+    <row r="35" spans="1:42" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>27</v>
       </c>
@@ -2517,7 +2517,7 @@
       </c>
       <c r="AP35" s="10"/>
     </row>
-    <row r="36" spans="1:42">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="H36" s="10"/>
@@ -2542,7 +2542,7 @@
       <c r="AO36" s="10"/>
       <c r="AP36" s="10"/>
     </row>
-    <row r="37" spans="1:42">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="AP37" s="10"/>
     </row>
-    <row r="38" spans="1:42">
+    <row r="38" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2708,7 +2708,7 @@
       </c>
       <c r="AP38" s="10"/>
     </row>
-    <row r="39" spans="1:42">
+    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="H39" s="10"/>
@@ -2733,7 +2733,7 @@
       <c r="AO39" s="10"/>
       <c r="AP39" s="10"/>
     </row>
-    <row r="40" spans="1:42">
+    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>60</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:42">
+    <row r="41" spans="1:42" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>61</v>
       </c>
@@ -2787,14 +2787,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.375" customWidth="1"/>
-    <col min="2" max="2" width="10.375" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>45</v>
       </c>
@@ -2805,7 +2805,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Status Analyse & Entwurf-Dokumente angepasst
</commit_message>
<xml_diff>
--- a/Projektmanagement/Aufgaben.xlsx
+++ b/Projektmanagement/Aufgaben.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="67">
   <si>
     <t>UseCases erstellen</t>
   </si>
@@ -704,7 +704,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="Y21" sqref="Y21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -908,7 +908,7 @@
         <v>41544</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>42</v>
@@ -954,7 +954,7 @@
         <v>41554</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>43</v>
@@ -1098,7 +1098,7 @@
         <v>41554</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>43</v>
@@ -1362,7 +1362,7 @@
         <v>41556</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="6"/>
@@ -1510,7 +1510,7 @@
         <v>41557</v>
       </c>
       <c r="G15" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="6"/>
@@ -1743,6 +1743,9 @@
       <c r="F21" s="2">
         <v>41562</v>
       </c>
+      <c r="G21" t="s">
+        <v>66</v>
+      </c>
       <c r="H21" s="10"/>
       <c r="I21" s="6"/>
       <c r="J21" s="8"/>
@@ -1768,6 +1771,7 @@
       <c r="Z21" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AA21" s="10"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="8"/>
       <c r="AG21" s="10"/>
@@ -1797,6 +1801,9 @@
       <c r="F22" s="2">
         <v>41562</v>
       </c>
+      <c r="G22" t="s">
+        <v>66</v>
+      </c>
       <c r="H22" s="10"/>
       <c r="I22" s="6"/>
       <c r="J22" s="8"/>
@@ -1822,6 +1829,7 @@
       <c r="Z22" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AA22" s="10"/>
       <c r="AD22" s="6"/>
       <c r="AE22" s="8"/>
       <c r="AG22" s="10"/>
@@ -1851,6 +1859,9 @@
       <c r="F23" s="2">
         <v>41562</v>
       </c>
+      <c r="G23" t="s">
+        <v>66</v>
+      </c>
       <c r="H23" s="10"/>
       <c r="I23" s="6"/>
       <c r="J23" s="8"/>
@@ -1876,6 +1887,7 @@
       <c r="Z23" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AA23" s="10"/>
       <c r="AD23" s="6"/>
       <c r="AE23" s="8"/>
       <c r="AG23" s="10"/>
@@ -1930,6 +1942,7 @@
       <c r="Z24" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AA24" s="10"/>
       <c r="AD24" s="6"/>
       <c r="AE24" s="8"/>
       <c r="AG24" s="10"/>
@@ -1959,6 +1972,9 @@
       <c r="F25" s="2">
         <v>41562</v>
       </c>
+      <c r="G25" t="s">
+        <v>66</v>
+      </c>
       <c r="H25" s="10"/>
       <c r="I25" s="6"/>
       <c r="J25" s="8"/>
@@ -1984,6 +2000,7 @@
       <c r="Z25" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AA25" s="10"/>
       <c r="AD25" s="6"/>
       <c r="AE25" s="8"/>
       <c r="AG25" s="10"/>
@@ -2035,6 +2052,7 @@
       <c r="Z26" s="10" t="s">
         <v>43</v>
       </c>
+      <c r="AA26" s="10"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="8"/>
       <c r="AG26" s="10"/>

</xml_diff>